<commit_message>
Update AveragedCompleted_5Planilha Mulino-PCA - Carcinicultura e Piscicultura.xlsx
</commit_message>
<xml_diff>
--- a/data/AveragedCompleted_5Planilha Mulino-PCA - Carcinicultura e Piscicultura.xlsx
+++ b/data/AveragedCompleted_5Planilha Mulino-PCA - Carcinicultura e Piscicultura.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\GitHub\PCA_AquacultureSystem\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D502B043-EBE0-45FB-9D8F-826402F738E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C40FD2-146E-4A21-8DDD-7948CB294931}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="18451" windowHeight="10996" xr2:uid="{DEE516F9-ADFD-4C63-AF22-1265D4977E59}"/>
   </bookViews>
@@ -1149,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D670D1E5-35DE-40FA-9024-A7AF08E417FD}">
   <dimension ref="A1:AW19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AW17" sqref="D5:AW17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1733,9 +1733,18 @@
       <c r="Z5" s="15">
         <v>100</v>
       </c>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="15"/>
-      <c r="AC5" s="15"/>
+      <c r="AA5" s="22">
+        <f>AVERAGE(AA6:AA17)</f>
+        <v>91.389193506643608</v>
+      </c>
+      <c r="AB5" s="22">
+        <f>AVERAGE(AB6:AB17)</f>
+        <v>85.366401156913412</v>
+      </c>
+      <c r="AC5" s="22">
+        <f>AVERAGE(AC6:AC17)</f>
+        <v>80.588208879631523</v>
+      </c>
       <c r="AD5" s="15">
         <v>0</v>
       </c>

</xml_diff>